<commit_message>
update task 22 notifikasi
</commit_message>
<xml_diff>
--- a/ACC Bid.xlsx
+++ b/ACC Bid.xlsx
@@ -1,19 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22130"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\git\Acc_Bid\Acc_Bid\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\git\ACCBid-Mobile\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F44A7EF-EFC4-45E1-9B03-9A8998D6B815}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="task 18" sheetId="4" r:id="rId1"/>
     <sheet name="task 19" sheetId="5" r:id="rId2"/>
+    <sheet name="task 22" sheetId="6" r:id="rId3"/>
+    <sheet name="task 23" sheetId="7" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="16">
   <si>
     <t>expected</t>
   </si>
@@ -46,12 +49,39 @@
   </si>
   <si>
     <t>Upload gambar error</t>
+  </si>
+  <si>
+    <t>semua notif</t>
+  </si>
+  <si>
+    <t>hanya notif lelang</t>
+  </si>
+  <si>
+    <t>hanya notif akun</t>
+  </si>
+  <si>
+    <t>hanya notif aplikasi</t>
+  </si>
+  <si>
+    <t>cek_input</t>
+  </si>
+  <si>
+    <t>search_text</t>
+  </si>
+  <si>
+    <t>Bagaimana cara melakukan Topup?</t>
+  </si>
+  <si>
+    <t>fail</t>
+  </si>
+  <si>
+    <t>xx92923</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -104,7 +134,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -114,6 +144,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -393,11 +424,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="A4:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -441,7 +472,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -479,4 +510,110 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{636E4703-EF51-4754-9585-8C289EE35242}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15CF37A5-5F22-475B-8674-E41628400F88}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="A1:B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="32.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
task history + edit profil
</commit_message>
<xml_diff>
--- a/ACC Bid.xlsx
+++ b/ACC Bid.xlsx
@@ -1,22 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22325"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\git\ACCBid-Mobile\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F44A7EF-EFC4-45E1-9B03-9A8998D6B815}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5F77A5B-548E-487C-92F9-BA2354127153}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="task 18" sheetId="4" r:id="rId1"/>
     <sheet name="task 19" sheetId="5" r:id="rId2"/>
     <sheet name="task 22" sheetId="6" r:id="rId3"/>
     <sheet name="task 23" sheetId="7" r:id="rId4"/>
+    <sheet name="view history" sheetId="9" r:id="rId5"/>
+    <sheet name="edit profil" sheetId="8" r:id="rId6"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -28,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="33">
   <si>
     <t>expected</t>
   </si>
@@ -76,6 +78,57 @@
   </si>
   <si>
     <t>xx92923</t>
+  </si>
+  <si>
+    <t>edit</t>
+  </si>
+  <si>
+    <t>foto profil</t>
+  </si>
+  <si>
+    <t>no handphone</t>
+  </si>
+  <si>
+    <t>alamat ktp</t>
+  </si>
+  <si>
+    <t>tgl lahir</t>
+  </si>
+  <si>
+    <t>pekerjaan</t>
+  </si>
+  <si>
+    <t>varInput</t>
+  </si>
+  <si>
+    <t>Yogyakarta</t>
+  </si>
+  <si>
+    <t>Wiraswasta</t>
+  </si>
+  <si>
+    <t>11/11/1998</t>
+  </si>
+  <si>
+    <t>view</t>
+  </si>
+  <si>
+    <t>event sedang bejalan</t>
+  </si>
+  <si>
+    <t>event selesai</t>
+  </si>
+  <si>
+    <t>081325184829</t>
+  </si>
+  <si>
+    <t>085242869607</t>
+  </si>
+  <si>
+    <t>IMG_20200128_092536.jpg</t>
+  </si>
+  <si>
+    <t>12/01/2020</t>
   </si>
 </sst>
 </file>
@@ -134,7 +187,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -145,6 +198,8 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -575,7 +630,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15CF37A5-5F22-475B-8674-E41628400F88}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="A1:B4"/>
     </sheetView>
   </sheetViews>
@@ -616,4 +671,155 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9A51D05-DD1A-4734-902B-D7427BB4C81B}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7BEB531-1660-47B6-AECB-EF1D2A03177D}">
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.28515625" style="7" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>